<commit_message>
Initial commit - AdlibSearchQA project with ExtentReports, DataProviders, Applitools and UI tests
</commit_message>
<xml_diff>
--- a/testData/NinjaDataSheet.xlsx
+++ b/testData/NinjaDataSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10402"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shada\OneDrive\Documents\CloudBerry\Batches\Jan 2025\Day 17\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lennoxfernandes/eclipse-workspace/AdlibSearchQA/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E0E232-8207-4408-8864-BFC6938A1051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07679B6-DEB9-514B-B86F-433DAD4C676B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="8180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>username</t>
   </si>
@@ -33,41 +33,17 @@
     <t>password</t>
   </si>
   <si>
-    <t>goodmorning@gmail.com</t>
+    <t>lennox.fernandes@gmail.com</t>
   </si>
   <si>
-    <t>test@1234</t>
-  </si>
-  <si>
-    <t>test121@test.com</t>
-  </si>
-  <si>
-    <t>test123</t>
-  </si>
-  <si>
-    <t>sid@cloudberry.services</t>
-  </si>
-  <si>
-    <t>Test123</t>
-  </si>
-  <si>
-    <t>otisdog22@yahoo.com</t>
-  </si>
-  <si>
-    <t>1234QWERT</t>
-  </si>
-  <si>
-    <t>shalaka.dongre@gmail.com</t>
-  </si>
-  <si>
-    <t>Test123!</t>
+    <t>abc@123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,6 +65,14 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -107,15 +91,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -397,16 +384,16 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.26953125" customWidth="1"/>
-    <col min="2" max="2" width="17.1796875" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -414,48 +401,36 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{825AA5BE-AC6A-8D41-82F0-8CF87A2A3B2D}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{4AD758E1-B26D-E54B-93AC-E6D8E0DCBD7D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>